<commit_message>
Added directory for JIMI-JIS - appendix to paper.
</commit_message>
<xml_diff>
--- a/output/SNIP/SNIP_ourSNIP_NLIQ_xlsx.xlsx
+++ b/output/SNIP/SNIP_ourSNIP_NLIQ_xlsx.xlsx
@@ -476,7 +476,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="F2" sqref="F2:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -520,8 +520,8 @@
         <v>126</v>
       </c>
       <c r="F2" s="1">
-        <f xml:space="preserve"> D2/E2</f>
-        <v>16.349206349206348</v>
+        <f xml:space="preserve"> E2/D2</f>
+        <v>6.1165048543689322E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -541,8 +541,8 @@
         <v>427</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F30" si="0" xml:space="preserve"> D3/E3</f>
-        <v>1.0304449648711944</v>
+        <f t="shared" ref="F3:F30" si="0" xml:space="preserve"> E3/D3</f>
+        <v>0.97045454545454546</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -563,7 +563,7 @@
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>19.90295358649789</v>
+        <v>5.0243799024803901E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -584,7 +584,7 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>0.79078014184397161</v>
+        <v>1.2645739910313902</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -605,7 +605,7 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>0.78113207547169816</v>
+        <v>1.2801932367149758</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -626,7 +626,7 @@
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>2.2246696035242293</v>
+        <v>0.44950495049504952</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -647,7 +647,7 @@
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>2.5446685878962536</v>
+        <v>0.39297848244620609</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -668,7 +668,7 @@
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>3.9073226544622424</v>
+        <v>0.25592972181551976</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>2.6964285714285716</v>
+        <v>0.37086092715231789</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -710,7 +710,7 @@
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>1.3552631578947369</v>
+        <v>0.73786407766990292</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -731,7 +731,7 @@
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
-        <v>1.6157840083073729</v>
+        <v>0.61889460154241649</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -752,7 +752,7 @@
       </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
-        <v>1.5312190287413281</v>
+        <v>0.65307443365695794</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -773,7 +773,7 @@
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>7.9913793103448274</v>
+        <v>0.12513484358144553</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -794,7 +794,7 @@
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>1.8528794590813709</v>
+        <v>0.53970051591795642</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -815,7 +815,7 @@
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
-        <v>4.9223602484472053</v>
+        <v>0.20315457413249211</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -836,7 +836,7 @@
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
-        <v>48.65625</v>
+        <v>2.0552344251766216E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -857,7 +857,7 @@
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>3.5996140858658947</v>
+        <v>0.27780755829536319</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -878,7 +878,7 @@
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
-        <v>17.647058823529413</v>
+        <v>5.6666666666666664E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -899,7 +899,7 @@
       </c>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
-        <v>1.4507042253521127</v>
+        <v>0.68932038834951459</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -920,7 +920,7 @@
       </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>4.1533742331288339</v>
+        <v>0.24076809453471196</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -941,7 +941,7 @@
       </c>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
-        <v>0.52794060179757718</v>
+        <v>1.8941524796447076</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -962,7 +962,7 @@
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
-        <v>2.3199999999999998</v>
+        <v>0.43103448275862066</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -983,7 +983,7 @@
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
-        <v>1.4057771664374141</v>
+        <v>0.71135029354207435</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="F25" s="1">
         <f t="shared" si="0"/>
-        <v>3.1847133757961785</v>
+        <v>0.314</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -1025,7 +1025,7 @@
       </c>
       <c r="F26" s="1">
         <f t="shared" si="0"/>
-        <v>0.99570815450643779</v>
+        <v>1.0043103448275863</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="F27" s="1">
         <f t="shared" si="0"/>
-        <v>3.2979719188767551</v>
+        <v>0.30321665089877009</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="F28" s="1">
         <f t="shared" si="0"/>
-        <v>8.2282608695652169</v>
+        <v>0.12153236459709379</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="F29" s="1">
         <f t="shared" si="0"/>
-        <v>3.6984126984126986</v>
+        <v>0.27038626609442062</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="19" x14ac:dyDescent="0.25">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="F30" s="1">
         <f t="shared" si="0"/>
-        <v>2.3790523690773067</v>
+        <v>0.42033542976939203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>